<commit_message>
Excel for Update members updated
</commit_message>
<xml_diff>
--- a/test_files/Code_list_with_update_members.xlsx
+++ b/test_files/Code_list_with_update_members.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21723"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88ED32F4-37C8-424A-A38A-4ABB4012BFE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5BE83E8-6BDF-4032-BA35-1EFD1BCDB606}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="5" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="301">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -1562,10 +1562,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
+    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3005,11 +3008,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="101.85546875" customWidth="1"/>
+    <col min="2" max="2" width="117" customWidth="1"/>
+    <col min="5" max="5" width="95" customWidth="1"/>
+    <col min="6" max="6" width="125.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3060,7 +3067,7 @@
       <c r="D2" t="s">
         <v>263</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F2" t="s">
@@ -3099,7 +3106,7 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
         <v>82</v>
@@ -3121,7 +3128,7 @@
       <c r="A4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>267</v>
       </c>
       <c r="C4" t="s">
@@ -3130,7 +3137,7 @@
       <c r="D4" t="s">
         <v>269</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F4" t="s">
@@ -3168,8 +3175,8 @@
       <c r="E5" t="s">
         <v>92</v>
       </c>
-      <c r="F5" t="s">
-        <v>88</v>
+      <c r="F5" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="G5" t="s">
         <v>96</v>
@@ -3203,8 +3210,8 @@
       <c r="E6" t="s">
         <v>99</v>
       </c>
-      <c r="F6" t="s">
-        <v>95</v>
+      <c r="F6" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="G6" t="s">
         <v>103</v>
@@ -3239,7 +3246,7 @@
         <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
         <v>109</v>
@@ -3363,6 +3370,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{DF254490-5C6C-4228-8C5E-227CC752AF9C}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{A57D2E07-4E9B-4F32-8B2D-03279BAF116D}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{59DB3C04-BB79-4E39-9A94-B2511378AAED}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{1D3C5EFE-A07E-4A5F-ADB9-CBB3E1B75D5F}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{94DE9652-1F00-43CE-A438-D72DDCF042A3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3371,15 +3385,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="131.42578125" customWidth="1"/>
-    <col min="6" max="6" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" customWidth="1"/>
+    <col min="5" max="5" width="87.140625" customWidth="1"/>
+    <col min="6" max="6" width="100.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3538,8 +3553,8 @@
       <c r="E5" t="s">
         <v>140</v>
       </c>
-      <c r="F5">
-        <v>3</v>
+      <c r="F5" t="s">
+        <v>132</v>
       </c>
       <c r="G5" t="s">
         <v>96</v>

</xml_diff>